<commit_message>
Adds some experiments with the new Vitis toolchain
</commit_message>
<xml_diff>
--- a/VitisVisionDisparity/Measurements.xlsx
+++ b/VitisVisionDisparity/Measurements.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Cluster</t>
   </si>
@@ -21,39 +21,61 @@
     <t>Latency</t>
   </si>
   <si>
-    <t>Period</t>
+    <t xml:space="preserve">Period (ns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExecTime (ms)</t>
+  </si>
+  <si>
+    <t>outlined_fun_18</t>
+  </si>
+  <si>
+    <t>padarray4</t>
+  </si>
+  <si>
+    <t>computeSAD</t>
+  </si>
+  <si>
+    <t>integralImage2D2D</t>
+  </si>
+  <si>
+    <t>finalSAD</t>
   </si>
   <si>
     <t>findDisparity</t>
-  </si>
-  <si>
-    <t>computeSAD</t>
-  </si>
-  <si>
-    <t>integralImage2D2D</t>
-  </si>
-  <si>
-    <t>finalSAD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,7 +90,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -584,50 +611,117 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="17.00390625"/>
+    <col bestFit="1" min="2" max="2" width="9.7109375"/>
+    <col bestFit="1" min="3" max="3" width="10.28125"/>
+    <col bestFit="1" min="4" max="4" style="1" width="13.28125"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" t="s">
+    <row r="1" s="2" customFormat="1" ht="14.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>6.9960000000000004</v>
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5">
+        <v>925899938</v>
+      </c>
+      <c r="C2" s="5">
+        <v>7.2999999999999998</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D7" si="0">B2*C2*10^-6</f>
+        <v>6759.0695473999995</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>6.8010000000000002</v>
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
+        <v>581010</v>
+      </c>
+      <c r="C3" s="5">
+        <v>7.2999999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2413729999999994</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1161738</v>
       </c>
       <c r="C4">
-        <v>6.0179999999999998</v>
+        <v>7.2999999999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>8.4806874000000008</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>85366734</v>
       </c>
       <c r="C5">
-        <v>6.806</v>
-      </c>
+        <v>7.2999999999999998</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>623.17715819999989</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1127272</v>
+      </c>
+      <c r="C6">
+        <v>7.2999999999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>8.2290855999999994</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>40855423</v>
+      </c>
+      <c r="C7">
+        <v>7.2999999999999998</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>298.24458789999994</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>